<commit_message>
Added Excel write functionality
</commit_message>
<xml_diff>
--- a/data/emp_export.xlsx
+++ b/data/emp_export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Emp_Id</t>
   </si>
@@ -418,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
@@ -592,6 +592,52 @@
         <v>50000</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>9578821821</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H8">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>9578821821</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H9">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Added - Functoin to Upload date from excel to db
</commit_message>
<xml_diff>
--- a/data/emp_export.xlsx
+++ b/data/emp_export.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
   <si>
     <t>Emp_Id</t>
   </si>
@@ -418,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H19"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
@@ -638,6 +638,236 @@
         <v>50000</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>9578821821</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H10">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>9578821821</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H11">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>9578821821</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H12">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>9578821821</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H13">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>9578821821</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H14">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>114</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>9578821821</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H15">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>9578821821</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H16">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>9578821821</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H17">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>9578821821</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H18">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>9578821821</v>
+      </c>
+      <c r="D19">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40310</v>
+      </c>
+      <c r="H19">
+        <v>50000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>